<commit_message>
Tweets Test was added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Tweets/Tweets.xlsx
+++ b/src/test/resources/TestData/Tweets/Tweets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Id</t>
   </si>
@@ -35,7 +35,13 @@
     <t>IsValid</t>
   </si>
   <si>
-    <t>It's my FirstTweet!</t>
+    <t>It's my First Tweet!</t>
+  </si>
+  <si>
+    <t>It's my Second Tweet!</t>
+  </si>
+  <si>
+    <t>It's my Third Tweet!</t>
   </si>
 </sst>
 </file>
@@ -354,16 +360,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -390,6 +396,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>